<commit_message>
s pos voc staging point
</commit_message>
<xml_diff>
--- a/data-raw/COVID Dates.xlsx
+++ b/data-raw/COVID Dates.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="994" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -14,6 +14,8 @@
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$G$57</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$G$57</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Sheet1!$A$1:$G$57</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$A$1:$G$57</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Sheet1!$A$1:$G$57</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="89">
   <si>
     <t xml:space="preserve">Start date</t>
   </si>
@@ -66,6 +68,9 @@
     <t xml:space="preserve">Tracing stop</t>
   </si>
   <si>
+    <t xml:space="preserve">Initial attempts at contact tracing are abandoned after system overwhelmed</t>
+  </si>
+  <si>
     <t xml:space="preserve">VE day</t>
   </si>
   <si>
@@ -81,6 +86,9 @@
     <t xml:space="preserve">Dexamethasone</t>
   </si>
   <si>
+    <t xml:space="preserve">Dexamethasone approved for patients with COVID-19</t>
+  </si>
+  <si>
     <t xml:space="preserve">Easter</t>
   </si>
   <si>
@@ -246,10 +254,76 @@
     <t xml:space="preserve">Shielding ends in Wales</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">England 2</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">nd</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> lockdown ends</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">England tier system</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.bbc.co.uk/news/uk-55147938</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pfizer vaccinations started</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B.1.1.7 variant announced</t>
+  </si>
+  <si>
+    <t xml:space="preserve">South East England tier 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">School Xmas holidays</t>
+  </si>
+  <si>
+    <t xml:space="preserve">South East England tier 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UK 3rd Lockdown</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 Million vaccinated</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Schools reopen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Group of 6 resumes (planned)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Non essential shops reopen (planned)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pubs reopen (planned)</t>
   </si>
 </sst>
 </file>
@@ -260,7 +334,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="YYYY\-MM\-DD"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -282,6 +356,14 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -360,17 +442,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G58"/>
+  <dimension ref="A1:G70"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I39" activeCellId="0" sqref="I39"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E73" activeCellId="0" sqref="E73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="13.9030612244898"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.219387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="13.3622448979592"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -442,6 +524,9 @@
       <c r="E4" s="0" t="s">
         <v>12</v>
       </c>
+      <c r="F4" s="0" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="n">
@@ -455,7 +540,7 @@
         <v>2</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -470,10 +555,10 @@
         <v>2</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -488,7 +573,7 @@
         <v>2</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -503,7 +588,10 @@
         <v>2</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -520,7 +608,7 @@
         <v>2</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -535,7 +623,7 @@
         <v>3</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -544,13 +632,13 @@
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D11" s="0" t="n">
         <v>3</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -559,13 +647,13 @@
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D12" s="0" t="n">
         <v>3</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -580,10 +668,10 @@
         <v>3</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -594,13 +682,13 @@
         <v>43990</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D14" s="0" t="n">
         <v>3</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -609,13 +697,13 @@
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D15" s="0" t="n">
         <v>3</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -630,7 +718,7 @@
         <v>4</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -639,13 +727,13 @@
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D17" s="0" t="n">
         <v>3</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -660,7 +748,7 @@
         <v>4</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -675,7 +763,7 @@
         <v>5</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -690,10 +778,10 @@
         <v>5</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -702,13 +790,13 @@
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D21" s="0" t="n">
         <v>5</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -723,7 +811,7 @@
         <v>5</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -738,7 +826,7 @@
         <v>3</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -755,7 +843,7 @@
         <v>3</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -770,7 +858,7 @@
         <v>3</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -785,7 +873,7 @@
         <v>3</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -800,7 +888,7 @@
         <v>3</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -815,7 +903,7 @@
         <v>3</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -830,7 +918,7 @@
         <v>3</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -845,7 +933,7 @@
         <v>1</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -854,13 +942,13 @@
       </c>
       <c r="B31" s="2"/>
       <c r="C31" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D31" s="0" t="n">
         <v>2</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -869,13 +957,13 @@
       </c>
       <c r="B32" s="2"/>
       <c r="C32" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D32" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -884,13 +972,13 @@
       </c>
       <c r="B33" s="2"/>
       <c r="C33" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D33" s="0" t="n">
         <v>3</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -901,13 +989,13 @@
         <v>44075</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D34" s="0" t="n">
         <v>2</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -916,13 +1004,13 @@
       </c>
       <c r="B35" s="2"/>
       <c r="C35" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D35" s="0" t="n">
         <v>3</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -931,13 +1019,13 @@
       </c>
       <c r="B36" s="2"/>
       <c r="C36" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D36" s="0" t="n">
         <v>3</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -946,13 +1034,13 @@
       </c>
       <c r="B37" s="2"/>
       <c r="C37" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D37" s="0" t="n">
         <v>3</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -969,7 +1057,7 @@
         <v>2</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -984,7 +1072,7 @@
         <v>3</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -999,7 +1087,7 @@
         <v>3</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1014,7 +1102,7 @@
         <v>3</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1029,7 +1117,7 @@
         <v>1</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1046,7 +1134,7 @@
         <v>2</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1061,7 +1149,7 @@
         <v>3</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1076,7 +1164,7 @@
         <v>3</v>
       </c>
       <c r="E45" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1091,7 +1179,7 @@
         <v>3</v>
       </c>
       <c r="E46" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1106,7 +1194,7 @@
         <v>3</v>
       </c>
       <c r="E47" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1121,7 +1209,7 @@
         <v>3</v>
       </c>
       <c r="E48" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1136,7 +1224,7 @@
         <v>3</v>
       </c>
       <c r="E49" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1151,7 +1239,7 @@
         <v>3</v>
       </c>
       <c r="E50" s="0" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1166,7 +1254,7 @@
         <v>3</v>
       </c>
       <c r="E51" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1181,7 +1269,7 @@
         <v>3</v>
       </c>
       <c r="E52" s="0" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1196,7 +1284,7 @@
         <v>3</v>
       </c>
       <c r="E53" s="0" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1211,7 +1299,7 @@
         <v>3</v>
       </c>
       <c r="E54" s="0" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1222,13 +1310,13 @@
         <v>44136</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D55" s="0" t="n">
         <v>3</v>
       </c>
       <c r="E55" s="0" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1243,10 +1331,10 @@
         <v>3</v>
       </c>
       <c r="E56" s="0" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="G56" s="0" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1261,13 +1349,13 @@
         <v>3</v>
       </c>
       <c r="E57" s="0" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="G57" s="0" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="2" t="n">
         <v>44167</v>
       </c>
@@ -1276,13 +1364,182 @@
         <v>9</v>
       </c>
       <c r="D58" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E58" s="0" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="2" t="n">
+        <v>44167</v>
+      </c>
+      <c r="B59" s="2"/>
+      <c r="C59" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D59" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="E58" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="G58" s="0" t="s">
-        <v>74</v>
+      <c r="E59" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="G59" s="0" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="2" t="n">
+        <v>44173</v>
+      </c>
+      <c r="C60" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D60" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E60" s="0" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="2" t="n">
+        <v>44179</v>
+      </c>
+      <c r="C61" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D61" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E61" s="0" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="2" t="n">
+        <v>44181</v>
+      </c>
+      <c r="C62" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D62" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E62" s="0" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="2" t="n">
+        <v>44183</v>
+      </c>
+      <c r="C63" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D63" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E63" s="0" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="2" t="n">
+        <v>44184</v>
+      </c>
+      <c r="C64" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D64" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E64" s="0" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="2" t="n">
+        <v>44200</v>
+      </c>
+      <c r="C65" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D65" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E65" s="0" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="2" t="n">
+        <v>44231</v>
+      </c>
+      <c r="C66" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D66" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E66" s="0" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="2" t="n">
+        <v>44263</v>
+      </c>
+      <c r="C67" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D67" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E67" s="0" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="2" t="n">
+        <v>44284</v>
+      </c>
+      <c r="C68" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D68" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E68" s="0" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="2" t="n">
+        <v>44298</v>
+      </c>
+      <c r="C69" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D69" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E69" s="0" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="2" t="n">
+        <v>44333</v>
+      </c>
+      <c r="C70" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D70" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E70" s="0" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
big clean up stable branch
</commit_message>
<xml_diff>
--- a/data-raw/COVID Dates.xlsx
+++ b/data-raw/COVID Dates.xlsx
@@ -5,17 +5,18 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$G$57</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$G$57</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Sheet1!$A$1:$G$57</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$A$1:$G$57</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Sheet1!$A$1:$G$57</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$G$82</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$G$56</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Sheet1!$A$1:$G$56</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$A$1:$G$56</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Sheet1!$A$1:$G$56</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$G$56</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="109">
   <si>
     <t xml:space="preserve">Start date</t>
   </si>
@@ -56,24 +57,48 @@
     <t xml:space="preserve">Feb half term</t>
   </si>
   <si>
+    <t xml:space="preserve">Health</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tracing stop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Initial attempts at contact tracing are abandoned after system overwhelmed</t>
+  </si>
+  <si>
     <t xml:space="preserve">Policy</t>
   </si>
   <si>
+    <t xml:space="preserve">Travel ban</t>
+  </si>
+  <si>
     <t xml:space="preserve">Lockdown</t>
   </si>
   <si>
-    <t xml:space="preserve">Health</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tracing stop</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Initial attempts at contact tracing are abandoned after system overwhelmed</t>
+    <t xml:space="preserve">UK 1st lockdown</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Easter 2020</t>
   </si>
   <si>
     <t xml:space="preserve">VE day</t>
   </si>
   <si>
+    <t xml:space="preserve">Easing plan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Conditional plan for easing lockdown announced</t>
+  </si>
+  <si>
+    <t xml:space="preserve">News</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cummingsgate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spring bank holiday</t>
+  </si>
+  <si>
     <t xml:space="preserve">Remdesivir</t>
   </si>
   <si>
@@ -83,72 +108,66 @@
     <t xml:space="preserve">Tracing restart</t>
   </si>
   <si>
+    <t xml:space="preserve">6 people limit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Relaxation shielding</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.gov.uk/government/news/prime-minister-hails-resilience-of-shielders-as-restrictions-set-to-ease</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Schools</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Year 6 return</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Retail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Outdoor markets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anti-racism demos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Travel quarantine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">University</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Univerity summer term end</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Year 10 &amp; 12 return</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All shops reopen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Face mask for travel</t>
+  </si>
+  <si>
     <t xml:space="preserve">Dexamethasone</t>
   </si>
   <si>
     <t xml:space="preserve">Dexamethasone approved for patients with COVID-19</t>
   </si>
   <si>
-    <t xml:space="preserve">Easter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Travel ban</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Schools</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Year 6 return</t>
-  </si>
-  <si>
-    <t xml:space="preserve">News</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cummingsgate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Easing plan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Conditional plan for easing lockdown announced</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Anti-racism demos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Year 10 &amp; 12 return</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spring bank holiday</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Retail</t>
-  </si>
-  <si>
-    <t xml:space="preserve">All shops reopen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Face mask for travel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6 people limit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Relaxation shielding</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.gov.uk/government/news/prime-minister-hails-resilience-of-shielders-as-restrictions-set-to-ease</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Outdoor markets</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Travel quarantine</t>
-  </si>
-  <si>
     <t xml:space="preserve">Leicester local lockdown</t>
   </si>
   <si>
+    <t xml:space="preserve">End UK 1st lockdown</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hotels and bars reopen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">End summer term</t>
+  </si>
+  <si>
     <t xml:space="preserve">Luton local lockdown</t>
   </si>
   <si>
@@ -158,142 +177,112 @@
     <t xml:space="preserve">Bradford local lockdown</t>
   </si>
   <si>
+    <t xml:space="preserve">Shielding ends (excl Wales)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.bbc.co.uk/news/uk-53618776</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manchester local lockdown</t>
+  </si>
+  <si>
     <t xml:space="preserve">North of England local lockdown</t>
   </si>
   <si>
+    <t xml:space="preserve">Start autumn term (Scotland)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shielding ends in Wales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Start autumn term</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Testing capacity limited</t>
+  </si>
+  <si>
+    <t xml:space="preserve">North East England tier 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Start univerity term</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Level 4 alert</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Circuit breaker recommendation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Liverpool tier 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">University autumn term start</t>
+  </si>
+  <si>
+    <t xml:space="preserve">South Wales local lockdown</t>
+  </si>
+  <si>
+    <t xml:space="preserve">North Wales local lockdown</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Variants</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B.1.1.7 first seqeunces</t>
+  </si>
+  <si>
     <t xml:space="preserve">Bolton local lockdown</t>
   </si>
   <si>
     <t xml:space="preserve">Birmingham local lockdown</t>
   </si>
   <si>
-    <t xml:space="preserve">Hotels and bars reopen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">End summer term</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Start autumn term</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Start autumn term (Scotland)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Summer holiday</t>
-  </si>
-  <si>
-    <t xml:space="preserve">End univerity term</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Start univerity term</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Manchester local lockdown</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Testing capacity limited</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Level 4 alert</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Circuit breaker recommended</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Liverpool tier 2</t>
+    <t xml:space="preserve">London tier 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lancashire tier 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">North West England tier 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wales firebreak lockdown</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manchester tier 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">School autumn half term</t>
+  </si>
+  <si>
+    <t xml:space="preserve">South Yorkshire tier 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Warrington tier 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nottinghamshire tier 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">West yorkshire tier 3</t>
   </si>
   <si>
     <t xml:space="preserve">England 2nd lockdown</t>
   </si>
   <si>
-    <t xml:space="preserve">Wales firebreak lockdown</t>
-  </si>
-  <si>
-    <t xml:space="preserve">South Wales local lockdown</t>
-  </si>
-  <si>
-    <t xml:space="preserve">North Wales local lockdown</t>
-  </si>
-  <si>
-    <t xml:space="preserve">North East England tier 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">North West England tier 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">London tier 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Manchester tier 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Warrington tier 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nottinghamshire tier 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">West yorkshire tier 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lancashire tier 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">South Yorkshire tier 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">School half term</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shielding ends (excl Wales)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.bbc.co.uk/news/uk-53618776</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shielding ends in Wales</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">England 2</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">nd</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> lockdown ends</t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve">England tier system</t>
   </si>
   <si>
+    <t xml:space="preserve">England 2nd lockdown ends</t>
+  </si>
+  <si>
     <t xml:space="preserve">https://www.bbc.co.uk/news/uk-55147938</t>
   </si>
   <si>
-    <t xml:space="preserve">Pfizer vaccinations started</t>
+    <t xml:space="preserve">Vaccination programme starts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">University autumn term end</t>
   </si>
   <si>
     <t xml:space="preserve">B.1.1.7 variant announced</t>
@@ -302,7 +291,7 @@
     <t xml:space="preserve">South East England tier 3</t>
   </si>
   <si>
-    <t xml:space="preserve">School Xmas holidays</t>
+    <t xml:space="preserve">End autumn term</t>
   </si>
   <si>
     <t xml:space="preserve">South East England tier 4</t>
@@ -311,19 +300,61 @@
     <t xml:space="preserve">UK 3rd Lockdown</t>
   </si>
   <si>
+    <t xml:space="preserve">Start spring term (remote)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">University spring term start</t>
+  </si>
+  <si>
     <t xml:space="preserve">10 Million vaccinated</t>
   </si>
   <si>
     <t xml:space="preserve">Schools reopen</t>
   </si>
   <si>
-    <t xml:space="preserve">Group of 6 resumes (planned)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Non essential shops reopen (planned)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pubs reopen (planned)</t>
+    <t xml:space="preserve">B.1.617.2 first UK sequences</t>
+  </si>
+  <si>
+    <t xml:space="preserve">University spring term end</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Roadmap step 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">End of stay at home order</t>
+  </si>
+  <si>
+    <t xml:space="preserve">End spring term</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Roadmap step 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Non essential shops reopen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Start summer term</t>
+  </si>
+  <si>
+    <t xml:space="preserve">India added to red list</t>
+  </si>
+  <si>
+    <t xml:space="preserve">University summer term start</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Easter 2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B.1.617.2 upgraded to VOC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Roadmap step 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pubs reopen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">University summer term end</t>
   </si>
 </sst>
 </file>
@@ -334,7 +365,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="YYYY\-MM\-DD"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -356,14 +387,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <vertAlign val="superscript"/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -442,17 +465,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G70"/>
+  <dimension ref="A1:G82"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E73" activeCellId="0" sqref="E73"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A55" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D65" activeCellId="0" sqref="D65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="13.3622448979592"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.6785714285714"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.4081632653061"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="13.2295918367347"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -497,80 +520,79 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="n">
-        <v>43913</v>
+        <v>43902</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="0" t="s">
         <v>9</v>
       </c>
       <c r="D3" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>10</v>
       </c>
+      <c r="F3" s="0" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="n">
-        <v>43902</v>
+        <v>43906</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D4" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="0" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="n">
-        <v>43959</v>
+        <v>43913</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="0" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D5" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="n">
-        <v>43977</v>
-      </c>
-      <c r="B6" s="2"/>
+        <v>43931</v>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>43934</v>
+      </c>
       <c r="C6" s="0" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>2</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" s="0" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="n">
-        <v>43979</v>
+        <v>43959</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="0" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D7" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E7" s="0" t="s">
         <v>17</v>
@@ -578,14 +600,14 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="n">
-        <v>43998</v>
+        <v>43961</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D8" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E8" s="0" t="s">
         <v>18</v>
@@ -596,43 +618,41 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="n">
-        <v>43931</v>
-      </c>
-      <c r="B9" s="2" t="n">
-        <v>43934</v>
-      </c>
+        <v>43974</v>
+      </c>
+      <c r="B9" s="2"/>
       <c r="C9" s="0" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="D9" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="n">
-        <v>43906</v>
+        <v>43976</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="0" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D10" s="0" t="n">
         <v>3</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="n">
-        <v>43983</v>
+        <v>43977</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="0" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="D11" s="0" t="n">
         <v>3</v>
@@ -640,14 +660,17 @@
       <c r="E11" s="0" t="s">
         <v>23</v>
       </c>
+      <c r="F11" s="0" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="n">
-        <v>43974</v>
+        <v>43979</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="0" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="D12" s="0" t="n">
         <v>3</v>
@@ -658,11 +681,11 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="n">
-        <v>43961</v>
+        <v>43979</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="0" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D13" s="0" t="n">
         <v>3</v>
@@ -670,153 +693,150 @@
       <c r="E13" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="F13" s="0" t="s">
-        <v>27</v>
-      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="n">
-        <v>43988</v>
-      </c>
-      <c r="B14" s="2" t="n">
-        <v>43990</v>
-      </c>
+        <v>43981</v>
+      </c>
+      <c r="B14" s="2"/>
       <c r="C14" s="0" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D14" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E14" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="G14" s="0" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="n">
-        <v>43997</v>
+        <v>43983</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="0" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D15" s="0" t="n">
         <v>3</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="n">
-        <v>43976</v>
+        <v>43983</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="0" t="s">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="D16" s="0" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="n">
-        <v>43997</v>
-      </c>
-      <c r="B17" s="2"/>
+        <v>43988</v>
+      </c>
+      <c r="B17" s="2" t="n">
+        <v>43990</v>
+      </c>
       <c r="C17" s="0" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="D17" s="0" t="n">
         <v>3</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="n">
-        <v>43997</v>
+        <v>43990</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="0" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D18" s="0" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="n">
-        <v>43979</v>
+        <v>43993</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="0" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="D19" s="0" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="n">
-        <v>43981</v>
+        <v>43997</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="0" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="D20" s="0" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="G20" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="n">
-        <v>43983</v>
+        <v>43997</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="0" t="s">
         <v>31</v>
       </c>
       <c r="D21" s="0" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="n">
-        <v>43990</v>
+        <v>43997</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="0" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D22" s="0" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="n">
-        <v>44016</v>
+        <v>43998</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="0" t="s">
@@ -826,144 +846,153 @@
         <v>3</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
+      </c>
+      <c r="F23" s="0" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="n">
-        <v>44037</v>
-      </c>
-      <c r="B24" s="2" t="n">
-        <v>44044</v>
-      </c>
+        <v>44016</v>
+      </c>
+      <c r="B24" s="2"/>
       <c r="C24" s="0" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D24" s="0" t="n">
         <v>3</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="n">
-        <v>44037</v>
+        <v>44016</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="0" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D25" s="0" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
+      </c>
+      <c r="F25" s="0" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="n">
-        <v>44044</v>
+        <v>44029</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" s="0" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="D26" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="n">
-        <v>44048</v>
-      </c>
-      <c r="B27" s="2"/>
+        <v>44037</v>
+      </c>
+      <c r="B27" s="2" t="n">
+        <v>44044</v>
+      </c>
       <c r="C27" s="0" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D27" s="0" t="n">
         <v>3</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="n">
-        <v>44114</v>
+        <v>44037</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" s="0" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D28" s="0" t="n">
         <v>3</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="n">
-        <v>44119</v>
+        <v>44044</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" s="0" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D29" s="0" t="n">
         <v>3</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="n">
-        <v>44016</v>
+        <v>44044</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" s="0" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D30" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="G30" s="0" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="n">
-        <v>44029</v>
+        <v>44045</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" s="0" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D31" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="n">
-        <v>44075</v>
+        <v>44048</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" s="0" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="D32" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -972,92 +1001,93 @@
       </c>
       <c r="B33" s="2"/>
       <c r="C33" s="0" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D33" s="0" t="n">
         <v>3</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="n">
-        <v>44029</v>
-      </c>
-      <c r="B34" s="2" t="n">
-        <v>44075</v>
-      </c>
+        <v>44061</v>
+      </c>
+      <c r="B34" s="2"/>
       <c r="C34" s="0" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="D34" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E34" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="G34" s="0" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="n">
-        <v>43993</v>
+        <v>44075</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" s="0" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D35" s="0" t="n">
         <v>3</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="n">
-        <v>44094</v>
-      </c>
-      <c r="B36" s="2"/>
+        <v>44082</v>
+      </c>
+      <c r="B36" s="2" t="n">
+        <v>44101</v>
+      </c>
       <c r="C36" s="0" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="D36" s="0" t="n">
         <v>3</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="2" t="n">
-        <v>44045</v>
+        <v>44091</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" s="0" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D37" s="0" t="n">
         <v>3</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="2" t="n">
-        <v>44082</v>
-      </c>
-      <c r="B38" s="2" t="n">
-        <v>44101</v>
-      </c>
+        <v>44094</v>
+      </c>
+      <c r="B38" s="2"/>
       <c r="C38" s="0" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="D38" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1066,13 +1096,13 @@
       </c>
       <c r="B39" s="2"/>
       <c r="C39" s="0" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D39" s="0" t="n">
         <v>3</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1081,13 +1111,13 @@
       </c>
       <c r="B40" s="2"/>
       <c r="C40" s="0" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D40" s="0" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1096,45 +1126,42 @@
       </c>
       <c r="B41" s="2"/>
       <c r="C41" s="0" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D41" s="0" t="n">
         <v>3</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="2" t="n">
-        <v>44140</v>
-      </c>
-      <c r="B42" s="2"/>
+        <v>44095</v>
+      </c>
       <c r="C42" s="0" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="D42" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="2" t="n">
-        <v>44127</v>
-      </c>
-      <c r="B43" s="2" t="n">
-        <v>44144</v>
-      </c>
+        <v>44099</v>
+      </c>
+      <c r="B43" s="2"/>
       <c r="C43" s="0" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D43" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1143,58 +1170,57 @@
       </c>
       <c r="B44" s="2"/>
       <c r="C44" s="0" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D44" s="0" t="n">
         <v>3</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="2" t="n">
-        <v>44099</v>
-      </c>
-      <c r="B45" s="2"/>
+        <v>44105</v>
+      </c>
       <c r="C45" s="0" t="s">
-        <v>9</v>
+        <v>65</v>
       </c>
       <c r="D45" s="0" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E45" s="0" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="2" t="n">
-        <v>44091</v>
+        <v>44114</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" s="0" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D46" s="0" t="n">
         <v>3</v>
       </c>
       <c r="E46" s="0" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="2" t="n">
-        <v>44122</v>
+        <v>44119</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" s="0" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D47" s="0" t="n">
         <v>3</v>
       </c>
       <c r="E47" s="0" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1203,88 +1229,92 @@
       </c>
       <c r="B48" s="2"/>
       <c r="C48" s="0" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D48" s="0" t="n">
         <v>3</v>
       </c>
       <c r="E48" s="0" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="2" t="n">
-        <v>44127</v>
+        <v>44120</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" s="0" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D49" s="0" t="n">
         <v>3</v>
       </c>
       <c r="E49" s="0" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="2" t="n">
-        <v>44131</v>
+        <v>44122</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" s="0" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D50" s="0" t="n">
         <v>3</v>
       </c>
       <c r="E50" s="0" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="2" t="n">
-        <v>44132</v>
-      </c>
-      <c r="B51" s="2"/>
+        <v>44127</v>
+      </c>
+      <c r="B51" s="2" t="n">
+        <v>44144</v>
+      </c>
       <c r="C51" s="0" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D51" s="0" t="n">
         <v>3</v>
       </c>
       <c r="E51" s="0" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="2" t="n">
-        <v>44137</v>
+        <v>44127</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" s="0" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D52" s="0" t="n">
         <v>3</v>
       </c>
       <c r="E52" s="0" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="2" t="n">
-        <v>44120</v>
-      </c>
-      <c r="B53" s="2"/>
+        <v>44127</v>
+      </c>
+      <c r="B53" s="2" t="n">
+        <v>44136</v>
+      </c>
       <c r="C53" s="0" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="D53" s="0" t="n">
         <v>3</v>
       </c>
       <c r="E53" s="0" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1293,81 +1323,73 @@
       </c>
       <c r="B54" s="2"/>
       <c r="C54" s="0" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D54" s="0" t="n">
         <v>3</v>
       </c>
       <c r="E54" s="0" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="2" t="n">
-        <v>44127</v>
-      </c>
-      <c r="B55" s="2" t="n">
-        <v>44136</v>
-      </c>
+        <v>44131</v>
+      </c>
+      <c r="B55" s="2"/>
       <c r="C55" s="0" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="D55" s="0" t="n">
         <v>3</v>
       </c>
       <c r="E55" s="0" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="2" t="n">
-        <v>44044</v>
+        <v>44132</v>
       </c>
       <c r="B56" s="2"/>
       <c r="C56" s="0" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D56" s="0" t="n">
         <v>3</v>
       </c>
       <c r="E56" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="G56" s="0" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="2" t="n">
-        <v>44061</v>
+        <v>44137</v>
       </c>
       <c r="B57" s="2"/>
       <c r="C57" s="0" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D57" s="0" t="n">
         <v>3</v>
       </c>
       <c r="E57" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="G57" s="0" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="2" t="n">
-        <v>44167</v>
+        <v>44140</v>
       </c>
       <c r="B58" s="2"/>
       <c r="C58" s="0" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D58" s="0" t="n">
         <v>1</v>
       </c>
       <c r="E58" s="0" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1376,16 +1398,19 @@
       </c>
       <c r="B59" s="2"/>
       <c r="C59" s="0" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D59" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E59" s="0" t="s">
-        <v>76</v>
+        <v>80</v>
+      </c>
+      <c r="F59" s="0" t="s">
+        <v>81</v>
       </c>
       <c r="G59" s="0" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1393,130 +1418,130 @@
         <v>44173</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D60" s="0" t="n">
         <v>2</v>
       </c>
       <c r="E60" s="0" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="2" t="n">
-        <v>44179</v>
+        <v>44176</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="D61" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E61" s="0" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="2" t="n">
-        <v>44181</v>
+        <v>44179</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>9</v>
+        <v>65</v>
       </c>
       <c r="D62" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E62" s="0" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="2" t="n">
-        <v>44183</v>
+        <v>44181</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="D63" s="0" t="n">
         <v>3</v>
       </c>
       <c r="E63" s="0" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="2" t="n">
-        <v>44184</v>
+        <v>44183</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="D64" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E64" s="0" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="2" t="n">
-        <v>44200</v>
+        <v>44184</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D65" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E65" s="0" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="2" t="n">
-        <v>44231</v>
+        <v>44200</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D66" s="0" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E66" s="0" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="2" t="n">
-        <v>44263</v>
+        <v>44200</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D67" s="0" t="n">
         <v>3</v>
       </c>
       <c r="E67" s="0" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="2" t="n">
-        <v>44284</v>
+        <v>44200</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="D68" s="0" t="n">
         <v>3</v>
       </c>
       <c r="E68" s="0" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="2" t="n">
-        <v>44298</v>
+        <v>44231</v>
       </c>
       <c r="C69" s="0" t="s">
         <v>9</v>
@@ -1525,25 +1550,205 @@
         <v>3</v>
       </c>
       <c r="E69" s="0" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="2" t="n">
+        <v>44263</v>
+      </c>
+      <c r="C70" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D70" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E70" s="0" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="2" t="n">
+        <v>44273</v>
+      </c>
+      <c r="C71" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="D71" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E71" s="0" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="2" t="n">
+        <v>44281</v>
+      </c>
+      <c r="C72" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="D72" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E72" s="0" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="2" t="n">
+        <v>44284</v>
+      </c>
+      <c r="C73" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D73" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E73" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="F73" s="0" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="2" t="n">
+        <v>44288</v>
+      </c>
+      <c r="C74" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="D74" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E74" s="0" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="2" t="n">
+        <v>44298</v>
+      </c>
+      <c r="C75" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D75" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E75" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="F75" s="0" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="2" t="n">
+        <v>44302</v>
+      </c>
+      <c r="C76" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="D76" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E76" s="0" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="2" t="n">
+        <v>44309</v>
+      </c>
+      <c r="C77" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="D77" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E77" s="0" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="2" t="n">
+        <v>44312</v>
+      </c>
+      <c r="C78" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="D78" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E78" s="0" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="2" t="n">
+        <v>44318</v>
+      </c>
+      <c r="B79" s="2" t="n">
+        <v>44321</v>
+      </c>
+      <c r="C79" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D79" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E79" s="0" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="2" t="n">
+        <v>44323</v>
+      </c>
+      <c r="C80" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="D80" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E80" s="0" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="2" t="n">
         <v>44333</v>
       </c>
-      <c r="C70" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D70" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="E70" s="0" t="s">
-        <v>88</v>
+      <c r="C81" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D81" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E81" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="F81" s="0" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="2" t="n">
+        <v>44358</v>
+      </c>
+      <c r="C82" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="D82" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E82" s="0" t="s">
+        <v>108</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G57"/>
+  <autoFilter ref="A1:G82"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>